<commit_message>
pdd section 1 near complete
</commit_message>
<xml_diff>
--- a/Planning/HonsProgress.xlsx
+++ b/Planning/HonsProgress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hons-moorhouse-p\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14416085-405C-441F-AD63-835BA5DE982C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9899EB21-C058-4E80-9090-403186AF94C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,13 +157,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -446,20 +461,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:J19"/>
+  <dimension ref="B2:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="42.85546875" customWidth="1"/>
-    <col min="7" max="8" width="25.7109375" customWidth="1"/>
-    <col min="10" max="10" width="38.28515625" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="10" width="17.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="38.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,14 +495,16 @@
       <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1">
         <v>1</v>
@@ -503,8 +522,16 @@
       <c r="H3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I3" s="4">
+        <f>AVERAGE(H3:H9)</f>
+        <v>0.84285714285714286</v>
+      </c>
+      <c r="J3" s="4">
+        <f>AVERAGE(H3:H19)</f>
+        <v>0.50000000000000011</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1">
         <v>1</v>
@@ -522,8 +549,10 @@
       <c r="H4" s="2">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I4" s="5"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1">
         <v>1</v>
@@ -536,13 +565,15 @@
         <v>9</v>
       </c>
       <c r="G5" s="1">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="H5" s="2">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="5"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1">
         <v>1</v>
@@ -560,8 +591,10 @@
       <c r="H6" s="2">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I6" s="5"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1">
         <v>1</v>
@@ -579,8 +612,10 @@
       <c r="H7" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I7" s="5"/>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1">
         <v>1</v>
@@ -596,10 +631,12 @@
         <v>70</v>
       </c>
       <c r="H8" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+        <v>0.8</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1">
         <v>2</v>
@@ -611,10 +648,16 @@
       <c r="F9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G9" s="1">
+        <v>125</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1">
         <v>2</v>
@@ -626,10 +669,19 @@
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G10" s="1">
+        <v>95</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="I10" s="4">
+        <f>AVERAGE(H10:H15)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1">
         <v>2</v>
@@ -641,10 +693,16 @@
       <c r="F11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G11" s="1">
+        <v>257</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1">
         <v>2</v>
@@ -656,10 +714,16 @@
       <c r="F12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G12" s="1">
+        <v>95</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1">
         <v>2</v>
@@ -671,10 +735,16 @@
       <c r="F13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G13" s="1">
+        <v>70</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="I13" s="5"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1">
         <v>2</v>
@@ -686,10 +756,16 @@
       <c r="F14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G14" s="1">
+        <v>162</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1">
         <v>2</v>
@@ -701,10 +777,16 @@
       <c r="F15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G15" s="1">
+        <v>109</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1">
         <v>3</v>
@@ -716,10 +798,19 @@
       <c r="F16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G16" s="1">
+        <v>45</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="I16" s="4">
+        <f>AVERAGE(H16:H18)</f>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1">
         <v>3</v>
@@ -731,10 +822,16 @@
       <c r="F17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G17" s="1">
+        <v>93</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="I17" s="5"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1">
         <v>3</v>
@@ -746,10 +843,16 @@
       <c r="F18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1">
         <v>4</v>
@@ -762,11 +865,39 @@
         <v>23</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="2"/>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+      <c r="I19" s="7">
+        <f>H19</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:G3 G19 J2">
+  <mergeCells count="5">
+    <mergeCell ref="I3:I9"/>
+    <mergeCell ref="I10:I15"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="J3:J19"/>
+    <mergeCell ref="H2:J2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="G1:G1048576 K2">
     <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A8966FAD-A053-4453-9C4B-18922B78112F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G3 G19 K2">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -778,9 +909,7 @@
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3 G19 J2">
-    <cfRule type="dataBar" priority="6">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -791,6 +920,18 @@
           <x14:id>{EEFE0845-8BDF-4ABF-B7FC-A0AFC4A5FEBC}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H3 H19">
@@ -804,9 +945,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3 H19">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -817,21 +956,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576 J2">
-    <cfRule type="dataBar" priority="2">
-      <dataBar>
+  <conditionalFormatting sqref="C1:D1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
         <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{A8966FAD-A053-4453-9C4B-18922B78112F}</x14:id>
-        </ext>
-      </extLst>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
+  <conditionalFormatting sqref="I3:J3 I1:J1 I20:J1048576 I4:I19">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -848,6 +985,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A8966FAD-A053-4453-9C4B-18922B78112F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G1:G1048576 K2</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C6856C74-0D06-46C3-9BA8-0C36517EDAFD}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
@@ -856,9 +1004,6 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G2:G3 G19 J2</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{EEFE0845-8BDF-4ABF-B7FC-A0AFC4A5FEBC}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
@@ -867,18 +1012,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G2:G3 G19 J2</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{A8966FAD-A053-4453-9C4B-18922B78112F}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>G1:G1048576 J2</xm:sqref>
+          <xm:sqref>G2:G3 G19 K2</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
work on gantt charts and pdd sections 1, 2
</commit_message>
<xml_diff>
--- a/Planning/HonsProgress.xlsx
+++ b/Planning/HonsProgress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hons-moorhouse-p\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCAA6DFD-0A35-4700-9CDC-F1729F4ACBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2765F4-57B1-420A-B8BE-3E2CFAAC0536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>#A</t>
   </si>
@@ -191,6 +191,12 @@
   </si>
   <si>
     <t>5 - Very High</t>
+  </si>
+  <si>
+    <t>refer to rubric! I'm dev + research!</t>
+  </si>
+  <si>
+    <t>the real constraint is use of TC &amp; SP score</t>
   </si>
 </sst>
 </file>
@@ -805,7 +811,7 @@
   <dimension ref="B2:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,7 +820,7 @@
     <col min="5" max="5" width="21.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
     <col min="7" max="8" width="17.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="38.28515625" customWidth="1"/>
+    <col min="9" max="9" width="46.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
@@ -861,7 +867,7 @@
       </c>
       <c r="H3" s="19">
         <f>AVERAGE(F3:F19)</f>
-        <v>0.6</v>
+        <v>0.63823529411764712</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -928,7 +934,7 @@
       <c r="C7" s="1">
         <v>5</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="1">
@@ -939,6 +945,9 @@
       </c>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
+      <c r="I7" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -951,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="1">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="F8" s="2">
         <v>0.9</v>
@@ -977,7 +986,7 @@
       </c>
       <c r="G9" s="19">
         <f>AVERAGE(F9:F15)</f>
-        <v>0.61428571428571421</v>
+        <v>0.70714285714285718</v>
       </c>
       <c r="H9" s="19"/>
     </row>
@@ -988,14 +997,14 @@
       <c r="C10" s="1">
         <v>2</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="1">
-        <v>95</v>
+        <v>152</v>
       </c>
       <c r="F10" s="2">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
@@ -1014,7 +1023,7 @@
         <v>257</v>
       </c>
       <c r="F11" s="2">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
@@ -1033,7 +1042,7 @@
         <v>95</v>
       </c>
       <c r="F12" s="2">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
@@ -1071,7 +1080,7 @@
         <v>117</v>
       </c>
       <c r="F14" s="2">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
@@ -1116,8 +1125,11 @@
         <v>0.19999999999999998</v>
       </c>
       <c r="H16" s="19"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>3</v>
       </c>
@@ -1135,8 +1147,9 @@
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="19"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="20"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>3</v>
       </c>
@@ -1154,8 +1167,9 @@
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="19"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="20"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>4</v>
       </c>
@@ -1176,7 +1190,8 @@
       <c r="H19" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="I16:I18"/>
     <mergeCell ref="G16:G18"/>
     <mergeCell ref="H3:H19"/>
     <mergeCell ref="F2:H2"/>

</xml_diff>

<commit_message>
more work on PDD + docs ready for meeting
</commit_message>
<xml_diff>
--- a/Planning/HonsProgress.xlsx
+++ b/Planning/HonsProgress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hons-moorhouse-p\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2765F4-57B1-420A-B8BE-3E2CFAAC0536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038258C3-1A41-486E-8C91-28B03C74BDB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>#A</t>
   </si>
@@ -196,7 +196,10 @@
     <t>refer to rubric! I'm dev + research!</t>
   </si>
   <si>
-    <t>the real constraint is use of TC &amp; SP score</t>
+    <t>the real constraint is use of TC &amp; SP score?</t>
+  </si>
+  <si>
+    <t>or say I'm using Sbench bc im not a bioinformatician</t>
   </si>
 </sst>
 </file>
@@ -496,10 +499,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -811,7 +814,7 @@
   <dimension ref="B2:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B2" sqref="B2:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +823,8 @@
     <col min="5" max="5" width="21.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
     <col min="7" max="8" width="17.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="46.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="53.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
@@ -861,13 +865,13 @@
       <c r="F3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="20">
         <f>AVERAGE(F3:F8)</f>
         <v>0.88333333333333341</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="20">
         <f>AVERAGE(F3:F19)</f>
-        <v>0.63823529411764712</v>
+        <v>0.66176470588235303</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -881,13 +885,13 @@
         <v>6</v>
       </c>
       <c r="E4" s="1">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="F4" s="2">
         <v>0.8</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
@@ -905,8 +909,8 @@
       <c r="F5" s="2">
         <v>0.8</v>
       </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
@@ -924,8 +928,8 @@
       <c r="F6" s="2">
         <v>0.8</v>
       </c>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -943,8 +947,8 @@
       <c r="F7" s="2">
         <v>1</v>
       </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
       <c r="I7" s="1" t="s">
         <v>51</v>
       </c>
@@ -965,8 +969,11 @@
       <c r="F8" s="2">
         <v>0.9</v>
       </c>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -984,11 +991,11 @@
       <c r="F9" s="2">
         <v>0.8</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="20">
         <f>AVERAGE(F9:F15)</f>
-        <v>0.70714285714285718</v>
-      </c>
-      <c r="H9" s="19"/>
+        <v>0.76428571428571435</v>
+      </c>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
@@ -1006,8 +1013,8 @@
       <c r="F10" s="2">
         <v>0.7</v>
       </c>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
@@ -1020,13 +1027,13 @@
         <v>13</v>
       </c>
       <c r="E11" s="1">
-        <v>257</v>
+        <v>184</v>
       </c>
       <c r="F11" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
+        <v>0.7</v>
+      </c>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
@@ -1044,8 +1051,8 @@
       <c r="F12" s="2">
         <v>0.7</v>
       </c>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
@@ -1063,8 +1070,8 @@
       <c r="F13" s="2">
         <v>1</v>
       </c>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
@@ -1082,8 +1089,8 @@
       <c r="F14" s="2">
         <v>0.75</v>
       </c>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
@@ -1101,8 +1108,8 @@
       <c r="F15" s="2">
         <v>0.7</v>
       </c>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
@@ -1120,12 +1127,12 @@
       <c r="F16" s="2">
         <v>0.3</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="20">
         <f>AVERAGE(F16:F18)</f>
         <v>0.19999999999999998</v>
       </c>
-      <c r="H16" s="19"/>
-      <c r="I16" s="20" t="s">
+      <c r="H16" s="20"/>
+      <c r="I16" s="19" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1145,9 +1152,9 @@
       <c r="F17" s="2">
         <v>0.3</v>
       </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="20"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="19"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
@@ -1165,9 +1172,9 @@
       <c r="F18" s="2">
         <v>0</v>
       </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="20"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="19"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
@@ -1187,7 +1194,7 @@
         <f>F19</f>
         <v>0</v>
       </c>
-      <c r="H19" s="19"/>
+      <c r="H19" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
pdd section 3 + prep for meeting
</commit_message>
<xml_diff>
--- a/Planning/HonsProgress.xlsx
+++ b/Planning/HonsProgress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hons-moorhouse-p\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038258C3-1A41-486E-8C91-28B03C74BDB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDD0FE9-0117-4A11-85DF-7E657D525BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -814,7 +814,7 @@
   <dimension ref="B2:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H19"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
       </c>
       <c r="H3" s="20">
         <f>AVERAGE(F3:F19)</f>
-        <v>0.66176470588235303</v>
+        <v>0.69705882352941184</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -938,7 +938,7 @@
       <c r="C7" s="1">
         <v>5</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="1">
@@ -993,7 +993,7 @@
       </c>
       <c r="G9" s="20">
         <f>AVERAGE(F9:F15)</f>
-        <v>0.76428571428571435</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="H9" s="20"/>
     </row>
@@ -1011,7 +1011,7 @@
         <v>152</v>
       </c>
       <c r="F10" s="2">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
@@ -1023,14 +1023,14 @@
       <c r="C11" s="1">
         <v>3</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="1">
         <v>184</v>
       </c>
       <c r="F11" s="2">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
@@ -1049,7 +1049,7 @@
         <v>95</v>
       </c>
       <c r="F12" s="2">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="G16" s="20">
         <f>AVERAGE(F16:F18)</f>
-        <v>0.19999999999999998</v>
+        <v>0.35000000000000003</v>
       </c>
       <c r="H16" s="20"/>
       <c r="I16" s="19" t="s">
@@ -1147,10 +1147,10 @@
         <v>19</v>
       </c>
       <c r="E17" s="1">
-        <v>93</v>
+        <v>144</v>
       </c>
       <c r="F17" s="2">
-        <v>0.3</v>
+        <v>0.75</v>
       </c>
       <c r="G17" s="19"/>
       <c r="H17" s="20"/>
@@ -1163,7 +1163,7 @@
       <c r="C18" s="1">
         <v>3</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E18" s="1">

</xml_diff>

<commit_message>
started a task list as a table, other small PDD changes
</commit_message>
<xml_diff>
--- a/Planning/HonsProgress.xlsx
+++ b/Planning/HonsProgress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hons-moorhouse-p\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F35FCD-2EAF-4B2B-8675-9C985E9307D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EC17C8-D208-4E8A-A364-5E5113B1A941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t>#A</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Risks Mits</t>
   </si>
   <si>
-    <t>Resources Required</t>
-  </si>
-  <si>
     <t>Ethics Legal</t>
   </si>
   <si>
@@ -200,13 +197,19 @@
   </si>
   <si>
     <t>or say I'm using Sbench bc im not a bioinformatician</t>
+  </si>
+  <si>
+    <t>Quantity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,20 +232,36 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,8 +273,20 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAEDF1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -437,13 +468,89 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -461,43 +568,58 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -508,26 +630,35 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -811,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I19"/>
+  <dimension ref="B2:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,13 +971,13 @@
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
       <c r="I2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -865,13 +996,13 @@
       <c r="F3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="25">
         <f>AVERAGE(F3:F8)</f>
-        <v>0.88333333333333341</v>
-      </c>
-      <c r="H3" s="20">
-        <f>AVERAGE(F3:F19)</f>
-        <v>0.69705882352941184</v>
+        <v>0.9</v>
+      </c>
+      <c r="H3" s="25">
+        <f>AVERAGE(F3:F18)</f>
+        <v>0.69687499999999991</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -890,8 +1021,8 @@
       <c r="F4" s="2">
         <v>0.8</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
@@ -909,8 +1040,8 @@
       <c r="F5" s="2">
         <v>0.8</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
@@ -928,8 +1059,8 @@
       <c r="F6" s="2">
         <v>0.8</v>
       </c>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -938,19 +1069,19 @@
       <c r="C7" s="1">
         <v>5</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
       <c r="I7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
@@ -967,12 +1098,12 @@
         <v>108</v>
       </c>
       <c r="F8" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
+        <v>1</v>
+      </c>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
       <c r="I8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
@@ -991,11 +1122,11 @@
       <c r="F9" s="2">
         <v>0.8</v>
       </c>
-      <c r="G9" s="20">
-        <f>AVERAGE(F9:F15)</f>
-        <v>0.7857142857142857</v>
-      </c>
-      <c r="H9" s="20"/>
+      <c r="G9" s="25">
+        <f>AVERAGE(F9:F14)</f>
+        <v>0.75</v>
+      </c>
+      <c r="H9" s="25"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
@@ -1013,8 +1144,8 @@
       <c r="F10" s="2">
         <v>0.75</v>
       </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
@@ -1032,8 +1163,8 @@
       <c r="F11" s="2">
         <v>0.75</v>
       </c>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
@@ -1051,159 +1182,140 @@
       <c r="F12" s="2">
         <v>0.75</v>
       </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>2</v>
       </c>
       <c r="C13" s="1">
-        <v>5</v>
-      </c>
-      <c r="D13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="1">
-        <v>0</v>
+        <v>117</v>
       </c>
       <c r="F13" s="2">
-        <v>1</v>
-      </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
+        <v>0.75</v>
+      </c>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>2</v>
       </c>
       <c r="C14" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="1">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="F14" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
+        <v>0.7</v>
+      </c>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="1">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="F15" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="25">
+        <f>AVERAGE(F15:F17)</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H15" s="25"/>
+      <c r="I15" s="24" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>3</v>
       </c>
       <c r="C16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="1">
-        <v>45</v>
+        <v>144</v>
       </c>
       <c r="F16" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="G16" s="20">
-        <f>AVERAGE(F16:F18)</f>
-        <v>0.35000000000000003</v>
-      </c>
-      <c r="H16" s="20"/>
-      <c r="I16" s="19" t="s">
-        <v>50</v>
-      </c>
+        <v>0.75</v>
+      </c>
+      <c r="G16" s="24"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="24"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>3</v>
       </c>
       <c r="C17" s="1">
-        <v>2</v>
-      </c>
-      <c r="D17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="1">
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="F17" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="19"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="24"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="24"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C18" s="1">
-        <v>3</v>
-      </c>
-      <c r="D18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
+      <c r="E18" s="1"/>
       <c r="F18" s="2">
         <v>0</v>
       </c>
-      <c r="G18" s="19"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="19"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="1">
-        <v>4</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="2">
+      <c r="G18" s="4">
+        <f>F18</f>
         <v>0</v>
       </c>
-      <c r="G19" s="4">
-        <f>F19</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="20"/>
+      <c r="H18" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="G16:G18"/>
-    <mergeCell ref="H3:H19"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="H3:H18"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="G3:G8"/>
-    <mergeCell ref="G9:G15"/>
+    <mergeCell ref="G9:G14"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:C1048576">
     <cfRule type="colorScale" priority="2">
@@ -1231,7 +1343,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E3 E19 I2">
+  <conditionalFormatting sqref="E2:E3 E18 I2">
     <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
@@ -1269,7 +1381,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F3 F19">
+  <conditionalFormatting sqref="F2:F3 F18">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1291,7 +1403,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:H3 G1:H1 G20:H1048576 G16:G19 G9">
+  <conditionalFormatting sqref="G19:H1048576 G3:H3 G1:H1 G15:G18 G9">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -1335,7 +1447,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E2:E3 E19 I2</xm:sqref>
+          <xm:sqref>E2:E3 E18 I2</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1397,101 +1509,101 @@
   <sheetData>
     <row r="4" spans="7:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="23" t="s">
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="29"/>
+      <c r="K5" s="30"/>
+    </row>
+    <row r="6" spans="7:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="24"/>
-      <c r="K5" s="25"/>
-    </row>
-    <row r="6" spans="7:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="14" t="s">
+      <c r="J6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="K6" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="12" t="s">
+    </row>
+    <row r="7" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G7" s="31" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G7" s="26" t="s">
+      <c r="H7" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="I7" s="12">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7">
+        <v>2</v>
+      </c>
+      <c r="K7" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G8" s="32"/>
+      <c r="H8" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="13">
-        <v>1</v>
-      </c>
-      <c r="J7" s="8">
+      <c r="I8" s="17">
         <v>2</v>
       </c>
-      <c r="K7" s="9">
+      <c r="J8" s="6">
+        <v>4</v>
+      </c>
+      <c r="K8" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G9" s="32"/>
+      <c r="H9" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="17">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G8" s="27"/>
-      <c r="H8" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="18">
-        <v>2</v>
-      </c>
-      <c r="J8" s="7">
+      <c r="J9" s="6">
+        <v>6</v>
+      </c>
+      <c r="K9" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G10" s="32"/>
+      <c r="H10" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="17">
         <v>4</v>
       </c>
-      <c r="K8" s="10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G9" s="27"/>
-      <c r="H9" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="I9" s="18">
-        <v>3</v>
-      </c>
-      <c r="J9" s="7">
-        <v>6</v>
-      </c>
-      <c r="K9" s="10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G10" s="27"/>
-      <c r="H10" s="16" t="s">
+      <c r="J10" s="6">
+        <v>8</v>
+      </c>
+      <c r="K10" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="7:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G11" s="33"/>
+      <c r="H11" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="18">
-        <v>4</v>
-      </c>
-      <c r="J10" s="7">
-        <v>8</v>
-      </c>
-      <c r="K10" s="10">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="7:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G11" s="28"/>
-      <c r="H11" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" s="14">
+      <c r="I11" s="13">
         <v>5</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="10">
         <v>10</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="11">
         <v>15</v>
       </c>
     </row>
@@ -1519,10 +1631,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8A8AA7A-9DBC-4D46-8D80-9792F2BA605A}">
-  <dimension ref="F5:I15"/>
+  <dimension ref="F5:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,41 +1647,42 @@
   <sheetData>
     <row r="5" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="I6" s="1">
-        <v>5600</v>
+        <f>16*400</f>
+        <v>6400</v>
       </c>
     </row>
     <row r="7" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="I7" s="1">
         <v>2200</v>
@@ -1577,13 +1690,13 @@
     </row>
     <row r="8" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="I8" s="1">
         <v>144.36000000000001</v>
@@ -1591,13 +1704,13 @@
     </row>
     <row r="9" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="H9" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I9" s="1">
         <v>1718.64</v>
@@ -1605,13 +1718,13 @@
     </row>
     <row r="10" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G10" s="1">
         <v>1200</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I10" s="1">
         <v>1200</v>
@@ -1620,7 +1733,7 @@
     <row r="11" spans="6:9" x14ac:dyDescent="0.25">
       <c r="I11">
         <f>SUM(I6:I10)</f>
-        <v>10863</v>
+        <v>11663</v>
       </c>
     </row>
     <row r="15" spans="6:9" x14ac:dyDescent="0.25">
@@ -1628,7 +1741,105 @@
         <v>10863</v>
       </c>
     </row>
+    <row r="20" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="6:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="6:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="22">
+        <v>5600</v>
+      </c>
+    </row>
+    <row r="23" spans="6:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="22">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="24" spans="6:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F24" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I24" s="22">
+        <v>144.36000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="6:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I25" s="22">
+        <v>1718.64</v>
+      </c>
+    </row>
+    <row r="26" spans="6:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G26" s="22">
+        <v>1200</v>
+      </c>
+      <c r="H26" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="I26" s="22">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="27" spans="6:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="35"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="23">
+        <v>10863</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F27:H27"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
progress from yesterday on PDD
</commit_message>
<xml_diff>
--- a/Planning/HonsProgress.xlsx
+++ b/Planning/HonsProgress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hons-moorhouse-p\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69934C2-03A2-4CC0-91A1-4067C19ADD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AC9600-B215-4BCB-A5BC-6CAE1E597746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -954,7 +954,7 @@
   <dimension ref="B2:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="H3" s="25">
         <f>AVERAGE(F3:F18)</f>
-        <v>0.69687499999999991</v>
+        <v>0.70312499999999989</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -1246,11 +1246,11 @@
         <v>45</v>
       </c>
       <c r="F15" s="2">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="G15" s="25">
         <f>AVERAGE(F15:F17)</f>
-        <v>0.41666666666666669</v>
+        <v>0.45</v>
       </c>
       <c r="H15" s="25"/>
       <c r="I15" s="24" t="s">

</xml_diff>

<commit_message>
working on pdd - near complete
</commit_message>
<xml_diff>
--- a/Planning/HonsProgress.xlsx
+++ b/Planning/HonsProgress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hons-moorhouse-p\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AC9600-B215-4BCB-A5BC-6CAE1E597746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFBDAC1-084E-4219-BD17-DBD41843E778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="61">
   <si>
     <t>#A</t>
   </si>
@@ -209,6 +209,21 @@
   </si>
   <si>
     <t>full list of tasks</t>
+  </si>
+  <si>
+    <t>Refs Needed?</t>
+  </si>
+  <si>
+    <t>Maybe</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -218,7 +233,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,8 +284,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,6 +323,16 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -554,12 +593,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -669,9 +710,20 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -951,23 +1003,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I25"/>
+  <dimension ref="B2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="34.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="7" max="8" width="17.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="53.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="38.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="9" width="17.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="53.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -977,19 +1030,22 @@
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="G2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="26"/>
       <c r="H2" s="26"/>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="26"/>
+      <c r="K2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -999,22 +1055,25 @@
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="1">
         <v>42</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="25">
-        <f>AVERAGE(F3:F8)</f>
+      <c r="H3" s="25">
+        <f>AVERAGE(G3:G8)</f>
         <v>0.9</v>
       </c>
-      <c r="H3" s="25">
-        <f>AVERAGE(F3:F18)</f>
-        <v>0.70312499999999989</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I3" s="25">
+        <f>AVERAGE(G3:G18)</f>
+        <v>0.71249999999999991</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -1024,16 +1083,19 @@
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="1">
         <v>381</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>0.8</v>
       </c>
-      <c r="G4" s="25"/>
       <c r="H4" s="25"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I4" s="25"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1043,16 +1105,19 @@
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="1">
         <v>174</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>0.8</v>
       </c>
-      <c r="G5" s="25"/>
       <c r="H5" s="25"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I5" s="25"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>1</v>
       </c>
@@ -1062,16 +1127,19 @@
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="1">
         <v>297</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>0.8</v>
       </c>
-      <c r="G6" s="25"/>
       <c r="H6" s="25"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I6" s="25"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>1</v>
       </c>
@@ -1081,19 +1149,22 @@
       <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="1">
         <v>59</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>1</v>
       </c>
-      <c r="G7" s="25"/>
       <c r="H7" s="25"/>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="25"/>
+      <c r="K7" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>1</v>
       </c>
@@ -1103,19 +1174,22 @@
       <c r="D8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="1">
         <v>108</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>1</v>
       </c>
-      <c r="G8" s="25"/>
       <c r="H8" s="25"/>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="25"/>
+      <c r="K8" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>2</v>
       </c>
@@ -1125,19 +1199,22 @@
       <c r="D9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="1">
         <v>125</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>0.8</v>
       </c>
-      <c r="G9" s="25">
-        <f>AVERAGE(F9:F14)</f>
+      <c r="H9" s="25">
+        <f>AVERAGE(G9:G14)</f>
         <v>0.75</v>
       </c>
-      <c r="H9" s="25"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I9" s="25"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>2</v>
       </c>
@@ -1147,16 +1224,19 @@
       <c r="D10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="1">
         <v>152</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>0.75</v>
       </c>
-      <c r="G10" s="25"/>
       <c r="H10" s="25"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="25"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>2</v>
       </c>
@@ -1166,16 +1246,19 @@
       <c r="D11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="1">
         <v>184</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>0.75</v>
       </c>
-      <c r="G11" s="25"/>
       <c r="H11" s="25"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I11" s="25"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>2</v>
       </c>
@@ -1185,16 +1268,19 @@
       <c r="D12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="1">
         <v>95</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>0.75</v>
       </c>
-      <c r="G12" s="25"/>
       <c r="H12" s="25"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>2</v>
       </c>
@@ -1204,16 +1290,19 @@
       <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="1">
         <v>117</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
         <v>0.75</v>
       </c>
-      <c r="G13" s="25"/>
       <c r="H13" s="25"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="25"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>2</v>
       </c>
@@ -1223,16 +1312,19 @@
       <c r="D14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="1">
         <v>136</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>0.7</v>
       </c>
-      <c r="G14" s="25"/>
       <c r="H14" s="25"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I14" s="25"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>3</v>
       </c>
@@ -1242,22 +1334,25 @@
       <c r="D15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="1">
         <v>45</v>
       </c>
-      <c r="F15" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G15" s="25">
-        <f>AVERAGE(F15:F17)</f>
-        <v>0.45</v>
-      </c>
-      <c r="H15" s="25"/>
-      <c r="I15" s="24" t="s">
+      <c r="G15" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="H15" s="25">
+        <f>AVERAGE(G15:G17)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I15" s="25"/>
+      <c r="K15" s="24" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>3</v>
       </c>
@@ -1267,17 +1362,20 @@
       <c r="D16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="1">
         <v>144</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>0.75</v>
       </c>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="24"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H16" s="24"/>
+      <c r="I16" s="25"/>
+      <c r="K16" s="24"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>3</v>
       </c>
@@ -1287,17 +1385,20 @@
       <c r="D17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="1">
         <v>0</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>0</v>
       </c>
-      <c r="G17" s="24"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="24"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H17" s="24"/>
+      <c r="I17" s="25"/>
+      <c r="K17" s="24"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>4</v>
       </c>
@@ -1307,39 +1408,45 @@
       <c r="D18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="2">
+      <c r="E18" s="4"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="2">
         <v>0</v>
       </c>
-      <c r="G18" s="4">
-        <f>F18</f>
+      <c r="H18" s="4">
+        <f>G18</f>
         <v>0</v>
       </c>
-      <c r="H18" s="25"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I23" s="1" t="s">
+      <c r="I18" s="25"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E20" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I24" s="1" t="s">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I25" s="1" t="s">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="1" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="H3:H18"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="G3:G8"/>
-    <mergeCell ref="G9:G14"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="I3:I18"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="H3:H8"/>
+    <mergeCell ref="H9:H14"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:C1048576">
     <cfRule type="colorScale" priority="2">
@@ -1353,7 +1460,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576 I2">
+  <conditionalFormatting sqref="F1:F1048576 K2">
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
@@ -1367,7 +1474,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E3 E18 I2">
+  <conditionalFormatting sqref="F2:F3 F18 K2">
     <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
@@ -1393,7 +1500,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
+  <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1405,7 +1512,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F3 F18">
+  <conditionalFormatting sqref="G2:G3 G18">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1427,7 +1534,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G19:H1048576 G3:H3 G1:H1 G15:G18 G9">
+  <conditionalFormatting sqref="H19:I1048576 E19:E1048576 H3:I3 H1:I1 E1 H15:H18 H9">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -1452,7 +1559,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E1:E1048576 I2</xm:sqref>
+          <xm:sqref>F1:F1048576 K2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C6856C74-0D06-46C3-9BA8-0C36517EDAFD}">
@@ -1471,7 +1578,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E2:E3 E18 I2</xm:sqref>
+          <xm:sqref>F2:F3 F18 K2</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
pdd - pushing for a submission (est. 94% complete)
</commit_message>
<xml_diff>
--- a/Planning/HonsProgress.xlsx
+++ b/Planning/HonsProgress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hons-moorhouse-p\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFBDAC1-084E-4219-BD17-DBD41843E778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780F0F57-4E93-4DA7-A130-34158C7238B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="66">
   <si>
     <t>#A</t>
   </si>
@@ -224,6 +224,21 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Reviewed?</t>
+  </si>
+  <si>
+    <t>Background &amp; Purpose</t>
+  </si>
+  <si>
+    <t>Rationale &amp; Operation</t>
+  </si>
+  <si>
+    <t>Methodology &amp; Outcomes</t>
+  </si>
+  <si>
+    <t>WIP</t>
   </si>
 </sst>
 </file>
@@ -600,7 +615,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -671,15 +686,36 @@
     <xf numFmtId="8" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -709,15 +745,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1003,452 +1030,527 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:K25"/>
+  <dimension ref="B2:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="34.28515625" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="9" width="17.140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="53.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="38.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="11" width="17.140625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="53.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="I2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="K2" s="1" t="s">
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="M2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="F3" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="1">
+      <c r="H3" s="1">
         <v>42</v>
       </c>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
-      <c r="H3" s="25">
-        <f>AVERAGE(G3:G8)</f>
-        <v>0.9</v>
-      </c>
-      <c r="I3" s="25">
-        <f>AVERAGE(G3:G18)</f>
-        <v>0.71249999999999991</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="29">
+        <f>AVERAGE(I3:I8)</f>
+        <v>0.93333333333333324</v>
+      </c>
+      <c r="K3" s="29">
+        <f>AVERAGE(I3:I18)</f>
+        <v>0.9375</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="30"/>
+      <c r="D4" s="1">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="F4" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="1">
+      <c r="H4" s="1">
         <v>381</v>
       </c>
-      <c r="G4" s="2">
+      <c r="I4" s="2">
         <v>0.8</v>
       </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="30"/>
+      <c r="D5" s="1">
         <v>3</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="F5" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="1">
+      <c r="H5" s="1">
         <v>174</v>
       </c>
-      <c r="G5" s="2">
+      <c r="I5" s="2">
         <v>0.8</v>
       </c>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="30"/>
+      <c r="D6" s="1">
         <v>4</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="F6" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="1">
+      <c r="H6" s="1">
         <v>297</v>
       </c>
-      <c r="G6" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="30"/>
+      <c r="D7" s="1">
         <v>5</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="F7" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="1">
+      <c r="H7" s="1">
         <v>59</v>
       </c>
-      <c r="G7" s="2">
-        <v>1</v>
-      </c>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="K7" s="1" t="s">
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="M7" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="30"/>
+      <c r="D8" s="1">
         <v>6</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="F8" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="1">
         <v>108</v>
       </c>
-      <c r="G8" s="2">
-        <v>1</v>
-      </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="K8" s="1" t="s">
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="M8" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>2</v>
       </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C9" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="F9" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="1">
+      <c r="H9" s="1">
         <v>125</v>
       </c>
-      <c r="G9" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="H9" s="25">
-        <f>AVERAGE(G9:G14)</f>
-        <v>0.75</v>
-      </c>
-      <c r="I9" s="25"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I9" s="2">
+        <v>1</v>
+      </c>
+      <c r="J9" s="29">
+        <f>AVERAGE(I9:I14)</f>
+        <v>1</v>
+      </c>
+      <c r="K9" s="29"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>2</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="31"/>
+      <c r="D10" s="1">
         <v>2</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="F10" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="1">
+      <c r="H10" s="1">
         <v>152</v>
       </c>
-      <c r="G10" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="31"/>
+      <c r="D11" s="1">
         <v>3</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="F11" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="1">
+      <c r="H11" s="1">
         <v>184</v>
       </c>
-      <c r="G11" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I11" s="2">
+        <v>1</v>
+      </c>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="31"/>
+      <c r="D12" s="1">
         <v>4</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="37" t="s">
+      <c r="F12" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="1">
+      <c r="H12" s="1">
         <v>95</v>
       </c>
-      <c r="G12" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>2</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="31"/>
+      <c r="D13" s="1">
         <v>6</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="F13" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="1">
         <v>117</v>
       </c>
-      <c r="G13" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I13" s="2">
+        <v>1</v>
+      </c>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>2</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="31"/>
+      <c r="D14" s="1">
         <v>7</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="F14" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="1">
+      <c r="H14" s="1">
         <v>136</v>
       </c>
-      <c r="G14" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I14" s="2">
+        <v>1</v>
+      </c>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>3</v>
       </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="C15" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="F15" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="1">
+      <c r="H15" s="1">
         <v>45</v>
       </c>
-      <c r="G15" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="H15" s="25">
-        <f>AVERAGE(G15:G17)</f>
-        <v>0.5</v>
-      </c>
-      <c r="I15" s="25"/>
-      <c r="K15" s="24" t="s">
+      <c r="I15" s="2">
+        <v>1</v>
+      </c>
+      <c r="J15" s="29">
+        <f>AVERAGE(I15:I17)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="K15" s="29"/>
+      <c r="M15" s="33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>3</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="32"/>
+      <c r="D16" s="1">
         <v>2</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="37" t="s">
+      <c r="F16" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="1">
+      <c r="H16" s="1">
         <v>144</v>
       </c>
-      <c r="G16" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="H16" s="24"/>
-      <c r="I16" s="25"/>
-      <c r="K16" s="24"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I16" s="2">
+        <v>1</v>
+      </c>
+      <c r="J16" s="33"/>
+      <c r="K16" s="29"/>
+      <c r="M16" s="33"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>3</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="32"/>
+      <c r="D17" s="1">
         <v>3</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="39" t="s">
+      <c r="F17" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="1">
+      <c r="H17" s="1">
         <v>0</v>
       </c>
-      <c r="G17" s="2">
-        <v>0</v>
-      </c>
-      <c r="H17" s="24"/>
-      <c r="I17" s="25"/>
-      <c r="K17" s="24"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J17" s="33"/>
+      <c r="K17" s="29"/>
+      <c r="M17" s="33"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>4</v>
       </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="2">
-        <v>0</v>
-      </c>
-      <c r="H18" s="4">
-        <f>G18</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="25"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E20" s="3" t="s">
+      <c r="F18"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="J18" s="4">
+        <f>I18</f>
+        <v>0.9</v>
+      </c>
+      <c r="K18" s="29"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G20" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K23" s="1" t="s">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M23" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K24" s="1" t="s">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M24" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K25" s="1" t="s">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M25" s="1" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="K15:K17"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="I3:I18"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="H3:H8"/>
-    <mergeCell ref="H9:H14"/>
+  <mergeCells count="9">
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="M15:M17"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="K3:K18"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="J3:J8"/>
+    <mergeCell ref="J9:J14"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="C9:C14"/>
   </mergeCells>
-  <conditionalFormatting sqref="B1:C1048576">
+  <conditionalFormatting sqref="B1:D3 B15:D15 B4:B14 D4:D14 C9 B18:D1048576 B16:B17 D16:D17">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1460,7 +1562,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576 K2">
+  <conditionalFormatting sqref="H1:H1048576 M2">
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
@@ -1474,7 +1576,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F3 F18 K2">
+  <conditionalFormatting sqref="H2:H3 H18 M2">
     <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
@@ -1500,7 +1602,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
+  <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1512,7 +1614,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3 G18">
+  <conditionalFormatting sqref="I2:I3 I18">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1534,7 +1636,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H19:I1048576 E19:E1048576 H3:I3 H1:I1 E1 H15:H18 H9">
+  <conditionalFormatting sqref="J19:K1048576 G19:G1048576 J3:K3 J1:K1 G1 J15:J18 J9">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -1559,7 +1661,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F1:F1048576 K2</xm:sqref>
+          <xm:sqref>H1:H1048576 M2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C6856C74-0D06-46C3-9BA8-0C36517EDAFD}">
@@ -1578,7 +1680,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F2:F3 F18 K2</xm:sqref>
+          <xm:sqref>H2:H3 H18 M2</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1640,17 +1742,17 @@
   <sheetData>
     <row r="4" spans="7:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="28" t="s">
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="29"/>
-      <c r="K5" s="30"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="37"/>
     </row>
     <row r="6" spans="7:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
       <c r="I6" s="13" t="s">
         <v>40</v>
       </c>
@@ -1662,7 +1764,7 @@
       </c>
     </row>
     <row r="7" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="38" t="s">
         <v>43</v>
       </c>
       <c r="H7" s="14" t="s">
@@ -1679,7 +1781,7 @@
       </c>
     </row>
     <row r="8" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G8" s="32"/>
+      <c r="G8" s="39"/>
       <c r="H8" s="15" t="s">
         <v>45</v>
       </c>
@@ -1694,7 +1796,7 @@
       </c>
     </row>
     <row r="9" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G9" s="32"/>
+      <c r="G9" s="39"/>
       <c r="H9" s="15" t="s">
         <v>46</v>
       </c>
@@ -1709,7 +1811,7 @@
       </c>
     </row>
     <row r="10" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G10" s="32"/>
+      <c r="G10" s="39"/>
       <c r="H10" s="15" t="s">
         <v>47</v>
       </c>
@@ -1724,7 +1826,7 @@
       </c>
     </row>
     <row r="11" spans="7:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G11" s="33"/>
+      <c r="G11" s="40"/>
       <c r="H11" s="16" t="s">
         <v>48</v>
       </c>
@@ -1958,11 +2060,11 @@
       </c>
     </row>
     <row r="27" spans="6:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F27" s="34" t="s">
+      <c r="F27" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="G27" s="35"/>
-      <c r="H27" s="36"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="43"/>
       <c r="I27" s="23">
         <v>10863</v>
       </c>

</xml_diff>

<commit_message>
PDD - submission ready
</commit_message>
<xml_diff>
--- a/Planning/HonsProgress.xlsx
+++ b/Planning/HonsProgress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hons-moorhouse-p\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780F0F57-4E93-4DA7-A130-34158C7238B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7BE924-CEFF-4DC2-B810-676D82133ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="61">
   <si>
     <t>#A</t>
   </si>
@@ -211,21 +211,9 @@
     <t>full list of tasks</t>
   </si>
   <si>
-    <t>Refs Needed?</t>
-  </si>
-  <si>
-    <t>Maybe</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Reviewed?</t>
   </si>
   <si>
@@ -236,9 +224,6 @@
   </si>
   <si>
     <t>Methodology &amp; Outcomes</t>
-  </si>
-  <si>
-    <t>WIP</t>
   </si>
 </sst>
 </file>
@@ -248,7 +233,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,13 +244,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -306,25 +284,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -343,11 +309,6 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -608,14 +569,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -629,128 +588,108 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="6" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="3" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1030,26 +969,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:M25"/>
+  <dimension ref="B2:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="17.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="28.5703125" customWidth="1"/>
-    <col min="6" max="6" width="22" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" customWidth="1"/>
-    <col min="10" max="11" width="17.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="53.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="38.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="1" customWidth="1"/>
+    <col min="7" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="10" width="17.85546875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="53.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1060,29 +997,26 @@
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="H2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="M2" s="1" t="s">
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="L2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="30" t="s">
-        <v>62</v>
+      <c r="C3" s="24" t="s">
+        <v>58</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -1090,169 +1024,153 @@
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="1">
         <v>59</v>
       </c>
-      <c r="G3" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" s="1">
-        <v>42</v>
-      </c>
-      <c r="I3" s="2">
-        <v>1</v>
-      </c>
-      <c r="J3" s="29">
-        <f>AVERAGE(I3:I8)</f>
-        <v>0.93333333333333324</v>
-      </c>
-      <c r="K3" s="29">
-        <f>AVERAGE(I3:I18)</f>
-        <v>0.9375</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3" s="26">
+        <f>AVERAGE(H3:H8)</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="26">
+        <f>AVERAGE(H3:H18)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="1">
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" s="1">
-        <v>381</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F4" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="1">
+        <f>241+175</f>
+        <v>416</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="30"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="1">
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="H5" s="1">
-        <v>174</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F5" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="1">
+        <v>157</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="30"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="1">
         <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="1">
-        <v>297</v>
-      </c>
-      <c r="I6" s="2">
-        <v>1</v>
-      </c>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F6" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="1">
+        <f>182+81</f>
+        <v>263</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="30"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="1">
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="H7" s="1">
-        <v>59</v>
-      </c>
-      <c r="I7" s="2">
-        <v>1</v>
-      </c>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="M7" s="1" t="s">
+      <c r="F7" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="1">
+        <v>77</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="L7" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="30"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="1">
         <v>6</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="F8" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="1">
         <v>108</v>
       </c>
-      <c r="I8" s="2">
-        <v>1</v>
-      </c>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="M8" s="1" t="s">
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="L8" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>2</v>
       </c>
-      <c r="C9" s="31" t="s">
-        <v>63</v>
+      <c r="C9" s="24" t="s">
+        <v>59</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -1260,160 +1178,144 @@
       <c r="E9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="1">
-        <v>125</v>
-      </c>
-      <c r="I9" s="2">
-        <v>1</v>
-      </c>
-      <c r="J9" s="29">
-        <f>AVERAGE(I9:I14)</f>
-        <v>1</v>
-      </c>
-      <c r="K9" s="29"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F9" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="1">
+        <v>120</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
+      <c r="I9" s="26">
+        <f>AVERAGE(H9:H14)</f>
+        <v>1</v>
+      </c>
+      <c r="J9" s="26"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>2</v>
       </c>
-      <c r="C10" s="31"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="1">
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" s="1">
-        <v>152</v>
-      </c>
-      <c r="I10" s="2">
-        <v>1</v>
-      </c>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F10" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="1">
+        <v>185</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="C11" s="31"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="1">
         <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="H11" s="1">
-        <v>184</v>
-      </c>
-      <c r="I11" s="2">
-        <v>1</v>
-      </c>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F11" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="1">
+        <f>63+110</f>
+        <v>173</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1</v>
+      </c>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="C12" s="31"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="1">
         <v>4</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="1">
-        <v>95</v>
-      </c>
-      <c r="I12" s="2">
-        <v>1</v>
-      </c>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F12" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>2</v>
       </c>
-      <c r="C13" s="31"/>
+      <c r="C13" s="24"/>
       <c r="D13" s="1">
         <v>6</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="1">
         <v>59</v>
       </c>
-      <c r="G13" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="H13" s="1">
-        <v>117</v>
-      </c>
-      <c r="I13" s="2">
-        <v>1</v>
-      </c>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>2</v>
       </c>
-      <c r="C14" s="31"/>
+      <c r="C14" s="24"/>
       <c r="D14" s="1">
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H14" s="1">
-        <v>136</v>
-      </c>
-      <c r="I14" s="2">
-        <v>1</v>
-      </c>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F14" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="1">
+        <f>42+53</f>
+        <v>95</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>3</v>
       </c>
-      <c r="C15" s="32" t="s">
-        <v>64</v>
+      <c r="C15" s="24" t="s">
+        <v>60</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -1421,82 +1323,73 @@
       <c r="E15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G15" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="H15" s="1">
-        <v>45</v>
-      </c>
-      <c r="I15" s="2">
-        <v>1</v>
-      </c>
-      <c r="J15" s="29">
-        <f>AVERAGE(I15:I17)</f>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="K15" s="29"/>
-      <c r="M15" s="33" t="s">
+      <c r="F15" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="1">
+        <v>75</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+      <c r="I15" s="26">
+        <f>AVERAGE(H15:H17)</f>
+        <v>1</v>
+      </c>
+      <c r="J15" s="26"/>
+      <c r="L15" s="25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>3</v>
       </c>
-      <c r="C16" s="32"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="1">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H16" s="1">
-        <v>144</v>
-      </c>
-      <c r="I16" s="2">
-        <v>1</v>
-      </c>
-      <c r="J16" s="33"/>
-      <c r="K16" s="29"/>
-      <c r="M16" s="33"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F16" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="1">
+        <v>156</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1</v>
+      </c>
+      <c r="I16" s="25"/>
+      <c r="J16" s="26"/>
+      <c r="L16" s="25"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>3</v>
       </c>
-      <c r="C17" s="32"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="1">
         <v>3</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="G17" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0</v>
-      </c>
-      <c r="I17" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="J17" s="33"/>
-      <c r="K17" s="29"/>
-      <c r="M17" s="33"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F17" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="1">
+        <v>223</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1</v>
+      </c>
+      <c r="I17" s="25"/>
+      <c r="J17" s="26"/>
+      <c r="L17" s="25"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>4</v>
       </c>
@@ -1507,46 +1400,40 @@
         <v>20</v>
       </c>
       <c r="F18"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="J18" s="4">
-        <f>I18</f>
-        <v>0.9</v>
-      </c>
-      <c r="K18" s="29"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="G20" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="M23" s="1" t="s">
+      <c r="G18" s="1"/>
+      <c r="H18" s="2">
+        <v>1</v>
+      </c>
+      <c r="I18" s="4">
+        <f>H18</f>
+        <v>1</v>
+      </c>
+      <c r="J18" s="26"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L23" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="M24" s="1" t="s">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L24" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="M25" s="1" t="s">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L25" s="1" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="C15:C17"/>
-    <mergeCell ref="M15:M17"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="K3:K18"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="J3:J8"/>
-    <mergeCell ref="J9:J14"/>
+    <mergeCell ref="L15:L17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J3:J18"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="I3:I8"/>
+    <mergeCell ref="I9:I14"/>
     <mergeCell ref="C3:C8"/>
     <mergeCell ref="C9:C14"/>
   </mergeCells>
@@ -1562,7 +1449,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576 M2">
+  <conditionalFormatting sqref="G1:G1048576 L2">
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
@@ -1576,7 +1463,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3 H18 M2">
+  <conditionalFormatting sqref="G2:G3 G18 L2">
     <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
@@ -1602,7 +1489,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I1048576">
+  <conditionalFormatting sqref="H1:H1048576">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1614,7 +1501,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3 I18">
+  <conditionalFormatting sqref="H2:H3 H18">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1636,7 +1523,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J19:K1048576 G19:G1048576 J3:K3 J1:K1 G1 J15:J18 J9">
+  <conditionalFormatting sqref="I19:J1048576 I3:J3 I1:J1 I15:I18 I9">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -1661,7 +1548,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H1:H1048576 M2</xm:sqref>
+          <xm:sqref>G1:G1048576 L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C6856C74-0D06-46C3-9BA8-0C36517EDAFD}">
@@ -1680,7 +1567,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H2:H3 H18 M2</xm:sqref>
+          <xm:sqref>G2:G3 G18 L2</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1742,101 +1629,101 @@
   <sheetData>
     <row r="4" spans="7:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="35" t="s">
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="36"/>
-      <c r="K5" s="37"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="31"/>
     </row>
     <row r="6" spans="7:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="13" t="s">
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="12">
-        <v>1</v>
-      </c>
-      <c r="J7" s="7">
+      <c r="I7" s="11">
+        <v>1</v>
+      </c>
+      <c r="J7" s="6">
         <v>2</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G8" s="39"/>
-      <c r="H8" s="15" t="s">
+      <c r="G8" s="33"/>
+      <c r="H8" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="16">
         <v>2</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <v>4</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="8">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G9" s="39"/>
-      <c r="H9" s="15" t="s">
+      <c r="G9" s="33"/>
+      <c r="H9" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="16">
         <v>3</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>6</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="8">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G10" s="39"/>
-      <c r="H10" s="15" t="s">
+      <c r="G10" s="33"/>
+      <c r="H10" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10" s="16">
         <v>4</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="5">
         <v>8</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="8">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="7:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G11" s="40"/>
-      <c r="H11" s="16" t="s">
+      <c r="G11" s="34"/>
+      <c r="H11" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="12">
         <v>5</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="9">
         <v>10</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="10">
         <v>15</v>
       </c>
     </row>
@@ -1976,96 +1863,96 @@
     </row>
     <row r="20" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="6:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F21" s="18" t="s">
+      <c r="F21" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="19" t="s">
+      <c r="H21" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="I21" s="19" t="s">
+      <c r="I21" s="18" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="6:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="20" t="s">
+      <c r="F22" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G22" s="21" t="s">
+      <c r="G22" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H22" s="21" t="s">
+      <c r="H22" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="22">
+      <c r="I22" s="21">
         <v>5600</v>
       </c>
     </row>
     <row r="23" spans="6:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="G23" s="21" t="s">
+      <c r="G23" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="H23" s="21" t="s">
+      <c r="H23" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="I23" s="22">
+      <c r="I23" s="21">
         <v>2200</v>
       </c>
     </row>
     <row r="24" spans="6:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F24" s="20" t="s">
+      <c r="F24" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="21" t="s">
+      <c r="G24" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="21" t="s">
+      <c r="H24" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="I24" s="22">
+      <c r="I24" s="21">
         <v>144.36000000000001</v>
       </c>
     </row>
     <row r="25" spans="6:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G25" s="21" t="s">
+      <c r="G25" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="H25" s="21" t="s">
+      <c r="H25" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="I25" s="22">
+      <c r="I25" s="21">
         <v>1718.64</v>
       </c>
     </row>
     <row r="26" spans="6:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G26" s="22">
+      <c r="G26" s="21">
         <v>1200</v>
       </c>
-      <c r="H26" s="21" t="s">
+      <c r="H26" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="I26" s="22">
+      <c r="I26" s="21">
         <v>1200</v>
       </c>
     </row>
     <row r="27" spans="6:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F27" s="41" t="s">
+      <c r="F27" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="G27" s="42"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="23">
+      <c r="G27" s="36"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="22">
         <v>10863</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made a first submission
</commit_message>
<xml_diff>
--- a/Planning/HonsProgress.xlsx
+++ b/Planning/HonsProgress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\hons-moorhouse-p\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7BE924-CEFF-4DC2-B810-676D82133ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F117536A-6773-4644-B1AB-FF77FA5C2579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -972,7 +972,7 @@
   <dimension ref="B2:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>